<commit_message>
ReAdd tags to PRIDE-compatible templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/2EXT02_Protein.xlsx
+++ b/templates/dataplant/2EXT02_Protein.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\nfdi4plants\SWATE_templates\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC591C7B-00BB-4975-B58E-E57AA438DE31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DDD09C-4B42-4475-8299-3B5940B70309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT02_Protein" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="145">
   <si>
     <t>Source Name</t>
   </si>
@@ -770,13 +770,13 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="164" formatCode="0.00\ &quot;pH&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;pH&quot;"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -816,10 +816,10 @@
     <tableColumn id="13" xr3:uid="{BDF38729-6075-4DDC-92EC-18B22F924A5B}" name="Term Source REF ()"/>
     <tableColumn id="14" xr3:uid="{4C48CDEB-E2A1-4229-B3BA-5B9AF1B61DC0}" name="Term Accession Number ()"/>
     <tableColumn id="22" xr3:uid="{A4D903B4-51B3-4426-B177-F00F2C25027C}" name="Parameter [extraction buffer]"/>
-    <tableColumn id="23" xr3:uid="{61C1498E-2253-4CED-81A0-CC5AFEF4F5FA}" name="Term Source REF (DPBO:0000050)" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{55D5CDBD-1BC8-4DEA-81C8-12338B1FB673}" name="Term Accession Number (DPBO:0000050)" dataDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{61C1498E-2253-4CED-81A0-CC5AFEF4F5FA}" name="Term Source REF (DPBO:0000050)" dataDxfId="2"/>
+    <tableColumn id="24" xr3:uid="{55D5CDBD-1BC8-4DEA-81C8-12338B1FB673}" name="Term Accession Number (DPBO:0000050)" dataDxfId="1"/>
     <tableColumn id="18" xr3:uid="{A76F4D4C-FBEC-4E1F-ABF1-313BBB6F55B7}" name="Parameter [pH]"/>
-    <tableColumn id="21" xr3:uid="{78B7D35C-7FA9-4BC4-BECD-4CD211088C0D}" name="Unit" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{78B7D35C-7FA9-4BC4-BECD-4CD211088C0D}" name="Unit" dataDxfId="0"/>
     <tableColumn id="19" xr3:uid="{8374D543-1198-4666-AE2A-72A23EA25666}" name="Term Source REF (UO:0000196)"/>
     <tableColumn id="20" xr3:uid="{411E97BD-0DF1-4D92-93D9-DDDF6560A10A}" name="Term Accession Number (UO:0000196)"/>
     <tableColumn id="30" xr3:uid="{BFA58742-E29B-43B4-B11E-3F4279DFD76B}" name="Parameter [sample pre-fractionation]"/>
@@ -1165,7 +1165,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1540,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8F898E-70F9-4443-B417-1E256527228F}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,7 +1552,7 @@
     <col min="2" max="2" width="57.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -1600,13 +1600,13 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -1614,25 +1614,25 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="7"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1645,30 +1645,35 @@
       <c r="D12" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>

</xml_diff>